<commit_message>
Fixed Trinity Delta description (relating to blast damage fix)
</commit_message>
<xml_diff>
--- a/Resources/Apexes.xlsx
+++ b/Resources/Apexes.xlsx
@@ -1623,9 +1623,6 @@
     <t>UHB Epsilon.png</t>
   </si>
   <si>
-    <t>The Darkfire shot upon Teleport arrival now deals Blast damage. (Blast damage is Armor Piercing if the darkfire shot hits the cockpit of armored invaders)</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=Fu2vK7lFLaY</t>
   </si>
   <si>
@@ -1993,6 +1990,9 @@
   </si>
   <si>
     <t>]</t>
+  </si>
+  <si>
+    <t>The Darkfire shot upon Teleport arrival now deals Blast damage</t>
   </si>
 </sst>
 </file>
@@ -2522,7 +2522,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N191"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="F128" sqref="F128"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
@@ -7895,7 +7897,7 @@
         <v>7</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>535</v>
+        <v>658</v>
       </c>
       <c r="G128" s="6">
         <v>20000</v>
@@ -7913,10 +7915,10 @@
         <v>175</v>
       </c>
       <c r="L128" s="22" t="s">
+        <v>535</v>
+      </c>
+      <c r="M128" s="22" t="s">
         <v>536</v>
-      </c>
-      <c r="M128" s="22" t="s">
-        <v>537</v>
       </c>
       <c r="N128" s="5"/>
     </row>
@@ -7955,10 +7957,10 @@
         <v>175</v>
       </c>
       <c r="L129" s="22" t="s">
+        <v>537</v>
+      </c>
+      <c r="M129" s="22" t="s">
         <v>538</v>
-      </c>
-      <c r="M129" s="22" t="s">
-        <v>539</v>
       </c>
       <c r="N129" s="5"/>
     </row>
@@ -7997,10 +7999,10 @@
         <v>31</v>
       </c>
       <c r="L130" s="22" t="s">
+        <v>539</v>
+      </c>
+      <c r="M130" s="22" t="s">
         <v>540</v>
-      </c>
-      <c r="M130" s="22" t="s">
-        <v>541</v>
       </c>
       <c r="N130" s="5"/>
     </row>
@@ -8039,10 +8041,10 @@
         <v>31</v>
       </c>
       <c r="L131" s="22" t="s">
+        <v>541</v>
+      </c>
+      <c r="M131" s="22" t="s">
         <v>542</v>
-      </c>
-      <c r="M131" s="22" t="s">
-        <v>543</v>
       </c>
       <c r="N131" s="5"/>
     </row>
@@ -8063,7 +8065,7 @@
         <v>38</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="G132" s="6">
         <v>10000</v>
@@ -8081,10 +8083,10 @@
         <v>44</v>
       </c>
       <c r="L132" s="22" t="s">
+        <v>544</v>
+      </c>
+      <c r="M132" s="22" t="s">
         <v>545</v>
-      </c>
-      <c r="M132" s="22" t="s">
-        <v>546</v>
       </c>
       <c r="N132" s="5"/>
     </row>
@@ -8123,10 +8125,10 @@
         <v>44</v>
       </c>
       <c r="L133" s="22" t="s">
+        <v>546</v>
+      </c>
+      <c r="M133" s="22" t="s">
         <v>547</v>
-      </c>
-      <c r="M133" s="22" t="s">
-        <v>548</v>
       </c>
       <c r="N133" s="5"/>
     </row>
@@ -8165,10 +8167,10 @@
         <v>147</v>
       </c>
       <c r="L134" s="22" t="s">
+        <v>548</v>
+      </c>
+      <c r="M134" s="22" t="s">
         <v>549</v>
-      </c>
-      <c r="M134" s="22" t="s">
-        <v>550</v>
       </c>
       <c r="N134" s="5"/>
     </row>
@@ -8207,10 +8209,10 @@
         <v>147</v>
       </c>
       <c r="L135" s="22" t="s">
+        <v>550</v>
+      </c>
+      <c r="M135" s="22" t="s">
         <v>551</v>
-      </c>
-      <c r="M135" s="22" t="s">
-        <v>552</v>
       </c>
       <c r="N135" s="5"/>
     </row>
@@ -8252,7 +8254,7 @@
         <v>205</v>
       </c>
       <c r="M136" s="22" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="N136" s="5"/>
     </row>
@@ -8291,10 +8293,10 @@
         <v>147</v>
       </c>
       <c r="L137" s="22" t="s">
+        <v>553</v>
+      </c>
+      <c r="M137" s="22" t="s">
         <v>554</v>
-      </c>
-      <c r="M137" s="22" t="s">
-        <v>555</v>
       </c>
       <c r="N137" s="5"/>
     </row>
@@ -8333,10 +8335,10 @@
         <v>20</v>
       </c>
       <c r="L138" s="22" t="s">
+        <v>555</v>
+      </c>
+      <c r="M138" s="22" t="s">
         <v>556</v>
-      </c>
-      <c r="M138" s="22" t="s">
-        <v>557</v>
       </c>
       <c r="N138" s="5"/>
     </row>
@@ -8375,10 +8377,10 @@
         <v>20</v>
       </c>
       <c r="L139" s="22" t="s">
+        <v>557</v>
+      </c>
+      <c r="M139" s="22" t="s">
         <v>558</v>
-      </c>
-      <c r="M139" s="22" t="s">
-        <v>559</v>
       </c>
       <c r="N139" s="5"/>
     </row>
@@ -8417,10 +8419,10 @@
         <v>147</v>
       </c>
       <c r="L140" s="22" t="s">
+        <v>559</v>
+      </c>
+      <c r="M140" s="22" t="s">
         <v>560</v>
-      </c>
-      <c r="M140" s="22" t="s">
-        <v>561</v>
       </c>
       <c r="N140" s="5"/>
     </row>
@@ -8459,10 +8461,10 @@
         <v>147</v>
       </c>
       <c r="L141" s="22" t="s">
+        <v>561</v>
+      </c>
+      <c r="M141" s="22" t="s">
         <v>562</v>
-      </c>
-      <c r="M141" s="22" t="s">
-        <v>563</v>
       </c>
       <c r="N141" s="5"/>
     </row>
@@ -8501,10 +8503,10 @@
         <v>44</v>
       </c>
       <c r="L142" s="22" t="s">
+        <v>563</v>
+      </c>
+      <c r="M142" s="22" t="s">
         <v>564</v>
-      </c>
-      <c r="M142" s="22" t="s">
-        <v>565</v>
       </c>
       <c r="N142" s="5"/>
     </row>
@@ -8543,10 +8545,10 @@
         <v>44</v>
       </c>
       <c r="L143" s="22" t="s">
+        <v>565</v>
+      </c>
+      <c r="M143" s="22" t="s">
         <v>566</v>
-      </c>
-      <c r="M143" s="22" t="s">
-        <v>567</v>
       </c>
       <c r="N143" s="5"/>
     </row>
@@ -8555,7 +8557,7 @@
         <v>72</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>10</v>
@@ -8585,7 +8587,7 @@
         <v>147</v>
       </c>
       <c r="L144" s="22" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="M144" s="22" t="s">
         <v>216</v>
@@ -8597,7 +8599,7 @@
         <v>72</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>32</v>
@@ -8627,7 +8629,7 @@
         <v>147</v>
       </c>
       <c r="L145" s="22" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="M145" s="22" t="s">
         <v>217</v>
@@ -8669,10 +8671,10 @@
         <v>13</v>
       </c>
       <c r="L146" s="22" t="s">
+        <v>570</v>
+      </c>
+      <c r="M146" s="22" t="s">
         <v>571</v>
-      </c>
-      <c r="M146" s="22" t="s">
-        <v>572</v>
       </c>
       <c r="N146" s="5"/>
     </row>
@@ -8711,10 +8713,10 @@
         <v>13</v>
       </c>
       <c r="L147" s="22" t="s">
+        <v>572</v>
+      </c>
+      <c r="M147" s="22" t="s">
         <v>573</v>
-      </c>
-      <c r="M147" s="22" t="s">
-        <v>574</v>
       </c>
       <c r="N147" s="5"/>
     </row>
@@ -8756,7 +8758,7 @@
         <v>237</v>
       </c>
       <c r="M148" s="22" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="N148" s="5"/>
     </row>
@@ -8795,10 +8797,10 @@
         <v>75</v>
       </c>
       <c r="L149" s="22" t="s">
+        <v>575</v>
+      </c>
+      <c r="M149" s="22" t="s">
         <v>576</v>
-      </c>
-      <c r="M149" s="22" t="s">
-        <v>577</v>
       </c>
       <c r="N149" s="5"/>
     </row>
@@ -8840,7 +8842,7 @@
         <v>222</v>
       </c>
       <c r="M150" s="22" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="N150" s="5"/>
     </row>
@@ -8879,10 +8881,10 @@
         <v>193</v>
       </c>
       <c r="L151" s="22" t="s">
+        <v>578</v>
+      </c>
+      <c r="M151" s="22" t="s">
         <v>579</v>
-      </c>
-      <c r="M151" s="22" t="s">
-        <v>580</v>
       </c>
       <c r="N151" s="5"/>
     </row>
@@ -8921,10 +8923,10 @@
         <v>13</v>
       </c>
       <c r="L152" s="12" t="s">
+        <v>580</v>
+      </c>
+      <c r="M152" s="22" t="s">
         <v>581</v>
-      </c>
-      <c r="M152" s="22" t="s">
-        <v>582</v>
       </c>
       <c r="N152" s="5"/>
     </row>
@@ -8963,10 +8965,10 @@
         <v>13</v>
       </c>
       <c r="L153" s="12" t="s">
+        <v>582</v>
+      </c>
+      <c r="M153" s="22" t="s">
         <v>583</v>
-      </c>
-      <c r="M153" s="22" t="s">
-        <v>584</v>
       </c>
       <c r="N153" s="5"/>
     </row>
@@ -9005,10 +9007,10 @@
         <v>147</v>
       </c>
       <c r="L154" s="22" t="s">
+        <v>584</v>
+      </c>
+      <c r="M154" s="22" t="s">
         <v>585</v>
-      </c>
-      <c r="M154" s="22" t="s">
-        <v>586</v>
       </c>
       <c r="N154" s="5"/>
     </row>
@@ -9047,10 +9049,10 @@
         <v>147</v>
       </c>
       <c r="L155" s="12" t="s">
+        <v>586</v>
+      </c>
+      <c r="M155" s="22" t="s">
         <v>587</v>
-      </c>
-      <c r="M155" s="22" t="s">
-        <v>588</v>
       </c>
       <c r="N155" s="5"/>
     </row>
@@ -9089,10 +9091,10 @@
         <v>31</v>
       </c>
       <c r="L156" s="22" t="s">
+        <v>588</v>
+      </c>
+      <c r="M156" s="22" t="s">
         <v>589</v>
-      </c>
-      <c r="M156" s="22" t="s">
-        <v>590</v>
       </c>
       <c r="N156" s="5"/>
     </row>
@@ -9131,10 +9133,10 @@
         <v>31</v>
       </c>
       <c r="L157" s="22" t="s">
+        <v>590</v>
+      </c>
+      <c r="M157" s="22" t="s">
         <v>591</v>
-      </c>
-      <c r="M157" s="22" t="s">
-        <v>592</v>
       </c>
       <c r="N157" s="5"/>
     </row>
@@ -9173,10 +9175,10 @@
         <v>147</v>
       </c>
       <c r="L158" s="22" t="s">
+        <v>592</v>
+      </c>
+      <c r="M158" s="22" t="s">
         <v>593</v>
-      </c>
-      <c r="M158" s="22" t="s">
-        <v>594</v>
       </c>
       <c r="N158" s="5"/>
     </row>
@@ -9215,10 +9217,10 @@
         <v>147</v>
       </c>
       <c r="L159" s="22" t="s">
+        <v>594</v>
+      </c>
+      <c r="M159" s="22" t="s">
         <v>595</v>
-      </c>
-      <c r="M159" s="22" t="s">
-        <v>596</v>
       </c>
       <c r="N159" s="5"/>
     </row>
@@ -9257,10 +9259,10 @@
         <v>20</v>
       </c>
       <c r="L160" s="22" t="s">
+        <v>596</v>
+      </c>
+      <c r="M160" s="22" t="s">
         <v>597</v>
-      </c>
-      <c r="M160" s="22" t="s">
-        <v>598</v>
       </c>
       <c r="N160" s="5"/>
     </row>
@@ -9299,10 +9301,10 @@
         <v>20</v>
       </c>
       <c r="L161" s="22" t="s">
+        <v>598</v>
+      </c>
+      <c r="M161" s="22" t="s">
         <v>599</v>
-      </c>
-      <c r="M161" s="22" t="s">
-        <v>600</v>
       </c>
       <c r="N161" s="5"/>
     </row>
@@ -9341,10 +9343,10 @@
         <v>252</v>
       </c>
       <c r="L162" s="22" t="s">
+        <v>600</v>
+      </c>
+      <c r="M162" s="32" t="s">
         <v>601</v>
-      </c>
-      <c r="M162" s="32" t="s">
-        <v>602</v>
       </c>
       <c r="N162" s="27" t="s">
         <v>254</v>
@@ -9385,10 +9387,10 @@
         <v>252</v>
       </c>
       <c r="L163" s="22" t="s">
+        <v>602</v>
+      </c>
+      <c r="M163" s="33" t="s">
         <v>603</v>
-      </c>
-      <c r="M163" s="33" t="s">
-        <v>604</v>
       </c>
       <c r="N163" s="27" t="s">
         <v>255</v>
@@ -9429,10 +9431,10 @@
         <v>75</v>
       </c>
       <c r="L164" s="22" t="s">
+        <v>604</v>
+      </c>
+      <c r="M164" s="33" t="s">
         <v>605</v>
-      </c>
-      <c r="M164" s="33" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="165" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -9470,10 +9472,10 @@
         <v>75</v>
       </c>
       <c r="L165" s="22" t="s">
+        <v>606</v>
+      </c>
+      <c r="M165" s="33" t="s">
         <v>607</v>
-      </c>
-      <c r="M165" s="33" t="s">
-        <v>608</v>
       </c>
       <c r="N165" s="27" t="s">
         <v>254</v>
@@ -9514,10 +9516,10 @@
         <v>20</v>
       </c>
       <c r="L166" t="s">
+        <v>608</v>
+      </c>
+      <c r="M166" s="33" t="s">
         <v>609</v>
-      </c>
-      <c r="M166" s="33" t="s">
-        <v>610</v>
       </c>
     </row>
     <row r="167" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -9555,10 +9557,10 @@
         <v>20</v>
       </c>
       <c r="L167" s="22" t="s">
+        <v>610</v>
+      </c>
+      <c r="M167" s="33" t="s">
         <v>611</v>
-      </c>
-      <c r="M167" s="33" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="168" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -9596,10 +9598,10 @@
         <v>44</v>
       </c>
       <c r="L168" s="22" t="s">
+        <v>612</v>
+      </c>
+      <c r="M168" s="33" t="s">
         <v>613</v>
-      </c>
-      <c r="M168" s="33" t="s">
-        <v>614</v>
       </c>
       <c r="N168" s="27" t="s">
         <v>254</v>
@@ -9640,10 +9642,10 @@
         <v>44</v>
       </c>
       <c r="L169" s="22" t="s">
+        <v>614</v>
+      </c>
+      <c r="M169" s="33" t="s">
         <v>615</v>
-      </c>
-      <c r="M169" s="33" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="170" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -9681,10 +9683,10 @@
         <v>252</v>
       </c>
       <c r="L170" t="s">
+        <v>616</v>
+      </c>
+      <c r="M170" s="33" t="s">
         <v>617</v>
-      </c>
-      <c r="M170" s="33" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="171" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -9722,10 +9724,10 @@
         <v>252</v>
       </c>
       <c r="L171" s="22" t="s">
+        <v>618</v>
+      </c>
+      <c r="M171" s="33" t="s">
         <v>619</v>
-      </c>
-      <c r="M171" s="33" t="s">
-        <v>620</v>
       </c>
     </row>
     <row r="172" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -9763,10 +9765,10 @@
         <v>75</v>
       </c>
       <c r="L172" s="22" t="s">
+        <v>620</v>
+      </c>
+      <c r="M172" s="33" t="s">
         <v>621</v>
-      </c>
-      <c r="M172" s="33" t="s">
-        <v>622</v>
       </c>
       <c r="N172" s="27" t="s">
         <v>255</v>
@@ -9807,10 +9809,10 @@
         <v>75</v>
       </c>
       <c r="L173" s="22" t="s">
+        <v>622</v>
+      </c>
+      <c r="M173" s="33" t="s">
         <v>623</v>
-      </c>
-      <c r="M173" s="33" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="174" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -9848,10 +9850,10 @@
         <v>147</v>
       </c>
       <c r="L174" s="22" t="s">
+        <v>624</v>
+      </c>
+      <c r="M174" s="33" t="s">
         <v>625</v>
-      </c>
-      <c r="M174" s="33" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="175" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -9889,10 +9891,10 @@
         <v>147</v>
       </c>
       <c r="L175" s="22" t="s">
+        <v>626</v>
+      </c>
+      <c r="M175" s="33" t="s">
         <v>627</v>
-      </c>
-      <c r="M175" s="33" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="176" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -9930,10 +9932,10 @@
         <v>31</v>
       </c>
       <c r="L176" s="22" t="s">
+        <v>628</v>
+      </c>
+      <c r="M176" s="33" t="s">
         <v>629</v>
-      </c>
-      <c r="M176" s="33" t="s">
-        <v>630</v>
       </c>
     </row>
     <row r="177" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -9971,10 +9973,10 @@
         <v>31</v>
       </c>
       <c r="L177" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="M177" s="33" t="s">
         <v>631</v>
-      </c>
-      <c r="M177" s="33" t="s">
-        <v>632</v>
       </c>
     </row>
     <row r="178" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -10015,7 +10017,7 @@
         <v>260</v>
       </c>
       <c r="M178" s="35" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="179" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -10053,10 +10055,10 @@
         <v>252</v>
       </c>
       <c r="L179" s="22" t="s">
+        <v>633</v>
+      </c>
+      <c r="M179" s="35" t="s">
         <v>634</v>
-      </c>
-      <c r="M179" s="35" t="s">
-        <v>635</v>
       </c>
       <c r="N179" s="27"/>
     </row>
@@ -10095,10 +10097,10 @@
         <v>147</v>
       </c>
       <c r="L180" s="22" t="s">
+        <v>635</v>
+      </c>
+      <c r="M180" s="35" t="s">
         <v>636</v>
-      </c>
-      <c r="M180" s="35" t="s">
-        <v>637</v>
       </c>
       <c r="N180" s="27"/>
     </row>
@@ -10137,10 +10139,10 @@
         <v>147</v>
       </c>
       <c r="L181" s="22" t="s">
+        <v>637</v>
+      </c>
+      <c r="M181" s="35" t="s">
         <v>638</v>
-      </c>
-      <c r="M181" s="35" t="s">
-        <v>639</v>
       </c>
       <c r="N181" s="27" t="s">
         <v>254</v>
@@ -10181,10 +10183,10 @@
         <v>147</v>
       </c>
       <c r="L182" t="s">
+        <v>639</v>
+      </c>
+      <c r="M182" s="35" t="s">
         <v>640</v>
-      </c>
-      <c r="M182" s="35" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="183" spans="1:14" ht="20.100000000000001" customHeight="1">
@@ -10222,7 +10224,7 @@
         <v>147</v>
       </c>
       <c r="M183" s="35" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="184" spans="1:14" ht="20.100000000000001" customHeight="1">
@@ -10242,7 +10244,7 @@
         <v>7</v>
       </c>
       <c r="F184" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="G184" s="34">
         <v>25000</v>
@@ -10254,16 +10256,16 @@
         <v>201</v>
       </c>
       <c r="J184" s="27" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="K184" s="27" t="s">
         <v>20</v>
       </c>
       <c r="L184" t="s">
+        <v>644</v>
+      </c>
+      <c r="M184" s="35" t="s">
         <v>645</v>
-      </c>
-      <c r="M184" s="35" t="s">
-        <v>646</v>
       </c>
     </row>
     <row r="185" spans="1:14" ht="20.100000000000001" customHeight="1">
@@ -10283,7 +10285,7 @@
         <v>6</v>
       </c>
       <c r="F185" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G185" s="34">
         <v>40000</v>
@@ -10295,16 +10297,16 @@
         <v>201</v>
       </c>
       <c r="J185" s="27" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="K185" s="27" t="s">
         <v>20</v>
       </c>
       <c r="L185" t="s">
+        <v>647</v>
+      </c>
+      <c r="M185" s="35" t="s">
         <v>648</v>
-      </c>
-      <c r="M185" s="35" t="s">
-        <v>649</v>
       </c>
     </row>
     <row r="186" spans="1:14" ht="20.100000000000001" customHeight="1">
@@ -10342,10 +10344,10 @@
         <v>252</v>
       </c>
       <c r="L186" t="s">
+        <v>649</v>
+      </c>
+      <c r="M186" s="35" t="s">
         <v>650</v>
-      </c>
-      <c r="M186" s="35" t="s">
-        <v>651</v>
       </c>
     </row>
     <row r="187" spans="1:14" ht="20.100000000000001" customHeight="1">
@@ -10383,10 +10385,10 @@
         <v>252</v>
       </c>
       <c r="L187" t="s">
+        <v>651</v>
+      </c>
+      <c r="M187" s="35" t="s">
         <v>652</v>
-      </c>
-      <c r="M187" s="35" t="s">
-        <v>653</v>
       </c>
     </row>
     <row r="188" spans="1:14" ht="20.100000000000001" customHeight="1">
@@ -10394,7 +10396,7 @@
         <v>94</v>
       </c>
       <c r="B188" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C188" t="s">
         <v>26</v>
@@ -10418,13 +10420,13 @@
         <v>202</v>
       </c>
       <c r="J188" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="K188" t="s">
         <v>31</v>
       </c>
       <c r="M188" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="189" spans="1:14" ht="20.100000000000001" customHeight="1">
@@ -10432,7 +10434,7 @@
         <v>94</v>
       </c>
       <c r="B189" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C189" t="s">
         <v>72</v>
@@ -10456,23 +10458,23 @@
         <v>202</v>
       </c>
       <c r="J189" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="K189" t="s">
         <v>31</v>
       </c>
       <c r="M189" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="190" spans="1:14" ht="20.100000000000001" customHeight="1">
       <c r="A190" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="191" spans="1:14" ht="20.100000000000001" customHeight="1">
       <c r="A191" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
   </sheetData>

</xml_diff>